<commit_message>
dodat random w1, azurirane neke greske
</commit_message>
<xml_diff>
--- a/doc/results/large_w0.xlsx
+++ b/doc/results/large_w0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="exact A2 vs exact A3" sheetId="1" r:id="rId1"/>
@@ -450,7 +450,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -466,13 +466,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -484,10 +496,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -496,8 +509,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -802,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -3885,10 +3903,14 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2:P2"/>
+      <selection activeCell="J2" sqref="J1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="8" width="8.88671875" style="5"/>
+    <col min="10" max="12" width="8.88671875" style="5"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
@@ -3897,16 +3919,16 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="J1" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
       <c r="N1" s="3" t="s">
         <v>107</v>
       </c>
@@ -3926,22 +3948,22 @@
       <c r="D2" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="5" t="s">
         <v>102</v>
       </c>
       <c r="N2" s="1" t="s">
@@ -3967,24 +3989,6 @@
       <c r="D3">
         <v>8</v>
       </c>
-      <c r="F3">
-        <v>22.140799999999999</v>
-      </c>
-      <c r="G3">
-        <v>1.0516900000000001E-3</v>
-      </c>
-      <c r="H3">
-        <v>26</v>
-      </c>
-      <c r="J3">
-        <v>18.914999999999999</v>
-      </c>
-      <c r="K3">
-        <v>9.0757100000000003E-4</v>
-      </c>
-      <c r="L3">
-        <v>19</v>
-      </c>
       <c r="N3">
         <v>3.21611</v>
       </c>
@@ -4008,24 +4012,6 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="F4">
-        <v>22.862100000000002</v>
-      </c>
-      <c r="G4">
-        <v>7.9737199999999997E-4</v>
-      </c>
-      <c r="H4">
-        <v>27</v>
-      </c>
-      <c r="J4">
-        <v>19.784500000000001</v>
-      </c>
-      <c r="K4">
-        <v>1.4528099999999999E-3</v>
-      </c>
-      <c r="L4">
-        <v>20</v>
-      </c>
       <c r="N4">
         <v>3.17564</v>
       </c>
@@ -4049,24 +4035,6 @@
       <c r="D5">
         <v>8</v>
       </c>
-      <c r="F5">
-        <v>20.067599999999999</v>
-      </c>
-      <c r="G5">
-        <v>1.6508499999999999E-3</v>
-      </c>
-      <c r="H5">
-        <v>21</v>
-      </c>
-      <c r="J5">
-        <v>20.9465</v>
-      </c>
-      <c r="K5">
-        <v>7.5271699999999997E-4</v>
-      </c>
-      <c r="L5">
-        <v>21</v>
-      </c>
       <c r="N5">
         <v>3.1515200000000001</v>
       </c>
@@ -4090,24 +4058,6 @@
       <c r="D6">
         <v>8</v>
       </c>
-      <c r="F6">
-        <v>23.7182</v>
-      </c>
-      <c r="G6">
-        <v>2.3881499999999999E-3</v>
-      </c>
-      <c r="H6">
-        <v>28</v>
-      </c>
-      <c r="J6">
-        <v>20.643599999999999</v>
-      </c>
-      <c r="K6">
-        <v>2.0763499999999998E-3</v>
-      </c>
-      <c r="L6">
-        <v>21</v>
-      </c>
       <c r="N6">
         <v>3.1151</v>
       </c>
@@ -4131,24 +4081,6 @@
       <c r="D7">
         <v>8</v>
       </c>
-      <c r="F7">
-        <v>23.4146</v>
-      </c>
-      <c r="G7">
-        <v>2.3539899999999998E-3</v>
-      </c>
-      <c r="H7">
-        <v>27</v>
-      </c>
-      <c r="J7">
-        <v>20.9268</v>
-      </c>
-      <c r="K7">
-        <v>1.05883E-3</v>
-      </c>
-      <c r="L7">
-        <v>21</v>
-      </c>
       <c r="N7">
         <v>3.0927799999999999</v>
       </c>
@@ -4172,24 +4104,6 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>2.5862099999999999</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>3</v>
-      </c>
-      <c r="J8">
-        <v>2.9310299999999998</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>3</v>
-      </c>
       <c r="N8">
         <v>1.2096800000000001</v>
       </c>
@@ -4213,24 +4127,6 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="F9">
-        <v>24.5745</v>
-      </c>
-      <c r="G9">
-        <v>1.3124899999999999E-3</v>
-      </c>
-      <c r="H9">
-        <v>29</v>
-      </c>
-      <c r="J9">
-        <v>20.625</v>
-      </c>
-      <c r="K9">
-        <v>1.0606299999999999E-3</v>
-      </c>
-      <c r="L9">
-        <v>21</v>
-      </c>
       <c r="N9">
         <v>3.0598999999999998</v>
       </c>
@@ -4253,24 +4149,6 @@
       </c>
       <c r="D10">
         <v>8</v>
-      </c>
-      <c r="F10">
-        <v>24.4178</v>
-      </c>
-      <c r="G10">
-        <v>1.33892E-3</v>
-      </c>
-      <c r="H10">
-        <v>29</v>
-      </c>
-      <c r="J10">
-        <v>20.9086</v>
-      </c>
-      <c r="K10">
-        <v>2.1335299999999998E-3</v>
-      </c>
-      <c r="L10">
-        <v>21</v>
       </c>
       <c r="N10">
         <v>3.0391699999999999</v>
@@ -4295,24 +4173,6 @@
       <c r="D11">
         <v>8</v>
       </c>
-      <c r="F11">
-        <v>25.576899999999998</v>
-      </c>
-      <c r="G11">
-        <v>1.40784E-3</v>
-      </c>
-      <c r="H11">
-        <v>30</v>
-      </c>
-      <c r="J11">
-        <v>21.776900000000001</v>
-      </c>
-      <c r="K11">
-        <v>1.17264E-3</v>
-      </c>
-      <c r="L11">
-        <v>22</v>
-      </c>
       <c r="N11">
         <v>3.0093800000000002</v>
       </c>
@@ -4336,24 +4196,6 @@
       <c r="D12">
         <v>8</v>
       </c>
-      <c r="F12">
-        <v>25.566700000000001</v>
-      </c>
-      <c r="G12">
-        <v>2.5776900000000001E-3</v>
-      </c>
-      <c r="H12">
-        <v>30</v>
-      </c>
-      <c r="J12">
-        <v>21.7683</v>
-      </c>
-      <c r="K12">
-        <v>2.3748100000000002E-3</v>
-      </c>
-      <c r="L12">
-        <v>22</v>
-      </c>
       <c r="N12">
         <v>2.9899100000000001</v>
       </c>
@@ -4376,24 +4218,6 @@
       </c>
       <c r="D13">
         <v>8</v>
-      </c>
-      <c r="F13">
-        <v>26.287099999999999</v>
-      </c>
-      <c r="G13">
-        <v>1.4737400000000001E-3</v>
-      </c>
-      <c r="H13">
-        <v>31</v>
-      </c>
-      <c r="J13">
-        <v>22.636099999999999</v>
-      </c>
-      <c r="K13">
-        <v>1.28291E-3</v>
-      </c>
-      <c r="L13">
-        <v>23</v>
       </c>
       <c r="N13">
         <v>2.9628399999999999</v>
@@ -4418,24 +4242,6 @@
       <c r="D14">
         <v>8</v>
       </c>
-      <c r="F14">
-        <v>23.0657</v>
-      </c>
-      <c r="G14">
-        <v>2.32921E-3</v>
-      </c>
-      <c r="H14">
-        <v>24</v>
-      </c>
-      <c r="J14">
-        <v>22.919699999999999</v>
-      </c>
-      <c r="K14">
-        <v>2.55404E-3</v>
-      </c>
-      <c r="L14">
-        <v>23</v>
-      </c>
       <c r="N14">
         <v>2.9476599999999999</v>
       </c>
@@ -4459,24 +4265,6 @@
       <c r="D15">
         <v>8</v>
       </c>
-      <c r="F15">
-        <v>22.9115</v>
-      </c>
-      <c r="G15">
-        <v>2.3492299999999999E-3</v>
-      </c>
-      <c r="H15">
-        <v>24</v>
-      </c>
-      <c r="J15">
-        <v>22.619599999999998</v>
-      </c>
-      <c r="K15">
-        <v>2.5871000000000002E-3</v>
-      </c>
-      <c r="L15">
-        <v>23</v>
-      </c>
       <c r="N15">
         <v>2.92292</v>
       </c>
@@ -4500,24 +4288,6 @@
       <c r="D16">
         <v>8</v>
       </c>
-      <c r="F16">
-        <v>27.425899999999999</v>
-      </c>
-      <c r="G16">
-        <v>2.9080400000000002E-3</v>
-      </c>
-      <c r="H16">
-        <v>32</v>
-      </c>
-      <c r="J16">
-        <v>22.903500000000001</v>
-      </c>
-      <c r="K16">
-        <v>2.6319300000000002E-3</v>
-      </c>
-      <c r="L16">
-        <v>23</v>
-      </c>
       <c r="N16">
         <v>2.9058999999999999</v>
       </c>
@@ -4541,24 +4311,6 @@
       <c r="D17">
         <v>8</v>
       </c>
-      <c r="F17">
-        <v>28</v>
-      </c>
-      <c r="G17">
-        <v>1.6634499999999999E-3</v>
-      </c>
-      <c r="H17">
-        <v>33</v>
-      </c>
-      <c r="J17">
-        <v>23.770800000000001</v>
-      </c>
-      <c r="K17">
-        <v>1.00216E-3</v>
-      </c>
-      <c r="L17">
-        <v>24</v>
-      </c>
       <c r="N17">
         <v>2.8833000000000002</v>
       </c>
@@ -4582,24 +4334,6 @@
       <c r="D18">
         <v>8</v>
       </c>
-      <c r="F18">
-        <v>27.9909</v>
-      </c>
-      <c r="G18">
-        <v>1.1757499999999999E-3</v>
-      </c>
-      <c r="H18">
-        <v>33</v>
-      </c>
-      <c r="J18">
-        <v>24.929400000000001</v>
-      </c>
-      <c r="K18">
-        <v>1.49222E-3</v>
-      </c>
-      <c r="L18">
-        <v>25</v>
-      </c>
       <c r="N18">
         <v>2.8673000000000002</v>
       </c>
@@ -4623,24 +4357,6 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="F19">
-        <v>2.8333300000000001</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>3</v>
-      </c>
       <c r="N19">
         <v>2.0181800000000001</v>
       </c>
@@ -4664,24 +4380,6 @@
       <c r="D20">
         <v>8</v>
       </c>
-      <c r="F20">
-        <v>29.002199999999998</v>
-      </c>
-      <c r="G20">
-        <v>3.4982799999999999E-3</v>
-      </c>
-      <c r="H20">
-        <v>34</v>
-      </c>
-      <c r="J20">
-        <v>24.63</v>
-      </c>
-      <c r="K20">
-        <v>3.0174500000000001E-3</v>
-      </c>
-      <c r="L20">
-        <v>25</v>
-      </c>
       <c r="N20">
         <v>2.8466100000000001</v>
       </c>
@@ -4705,24 +4403,6 @@
       <c r="D21">
         <v>8</v>
       </c>
-      <c r="F21">
-        <v>25.0596</v>
-      </c>
-      <c r="G21">
-        <v>2.7464E-3</v>
-      </c>
-      <c r="H21">
-        <v>26</v>
-      </c>
-      <c r="J21">
-        <v>24.913900000000002</v>
-      </c>
-      <c r="K21">
-        <v>2.9082000000000001E-3</v>
-      </c>
-      <c r="L21">
-        <v>25</v>
-      </c>
       <c r="N21">
         <v>2.8315199999999998</v>
       </c>
@@ -4746,24 +4426,6 @@
       <c r="D22">
         <v>8</v>
       </c>
-      <c r="F22">
-        <v>24.906500000000001</v>
-      </c>
-      <c r="G22">
-        <v>2.5106799999999999E-3</v>
-      </c>
-      <c r="H22">
-        <v>26</v>
-      </c>
-      <c r="J22">
-        <v>24.615200000000002</v>
-      </c>
-      <c r="K22">
-        <v>2.3292600000000001E-3</v>
-      </c>
-      <c r="L22">
-        <v>25</v>
-      </c>
       <c r="N22">
         <v>2.8125499999999999</v>
       </c>
@@ -4787,24 +4449,6 @@
       <c r="D23">
         <v>8</v>
       </c>
-      <c r="F23">
-        <v>29.704499999999999</v>
-      </c>
-      <c r="G23">
-        <v>3.74866E-3</v>
-      </c>
-      <c r="H23">
-        <v>35</v>
-      </c>
-      <c r="J23">
-        <v>24.8994</v>
-      </c>
-      <c r="K23">
-        <v>1.55685E-3</v>
-      </c>
-      <c r="L23">
-        <v>25</v>
-      </c>
       <c r="N23">
         <v>2.7982900000000002</v>
       </c>
@@ -4828,24 +4472,6 @@
       <c r="D24">
         <v>8</v>
       </c>
-      <c r="F24">
-        <v>25.765799999999999</v>
-      </c>
-      <c r="G24">
-        <v>1.48351E-3</v>
-      </c>
-      <c r="H24">
-        <v>27</v>
-      </c>
-      <c r="J24">
-        <v>25.765799999999999</v>
-      </c>
-      <c r="K24">
-        <v>1.6688300000000001E-3</v>
-      </c>
-      <c r="L24">
-        <v>26</v>
-      </c>
       <c r="N24">
         <v>2.78084</v>
       </c>
@@ -4869,24 +4495,6 @@
       <c r="D25">
         <v>8</v>
       </c>
-      <c r="F25">
-        <v>30.852399999999999</v>
-      </c>
-      <c r="G25">
-        <v>4.0934200000000004E-3</v>
-      </c>
-      <c r="H25">
-        <v>36</v>
-      </c>
-      <c r="J25">
-        <v>26.923100000000002</v>
-      </c>
-      <c r="K25">
-        <v>3.48388E-3</v>
-      </c>
-      <c r="L25">
-        <v>27</v>
-      </c>
       <c r="N25">
         <v>2.7692999999999999</v>
       </c>
@@ -4910,24 +4518,6 @@
       <c r="D26">
         <v>8</v>
       </c>
-      <c r="F26">
-        <v>26.625</v>
-      </c>
-      <c r="G26">
-        <v>1.5788499999999999E-3</v>
-      </c>
-      <c r="H26">
-        <v>28</v>
-      </c>
-      <c r="J26">
-        <v>26.625</v>
-      </c>
-      <c r="K26">
-        <v>3.2784300000000001E-3</v>
-      </c>
-      <c r="L26">
-        <v>27</v>
-      </c>
       <c r="N26">
         <v>2.7531699999999999</v>
       </c>
@@ -4951,24 +4541,6 @@
       <c r="D27">
         <v>8</v>
       </c>
-      <c r="F27">
-        <v>30.836400000000001</v>
-      </c>
-      <c r="G27">
-        <v>2.9244499999999999E-3</v>
-      </c>
-      <c r="H27">
-        <v>36</v>
-      </c>
-      <c r="J27">
-        <v>26.909099999999999</v>
-      </c>
-      <c r="K27">
-        <v>1.8363699999999999E-3</v>
-      </c>
-      <c r="L27">
-        <v>27</v>
-      </c>
       <c r="N27">
         <v>2.7402899999999999</v>
       </c>
@@ -4992,24 +4564,6 @@
       <c r="D28">
         <v>8</v>
       </c>
-      <c r="F28">
-        <v>32.282899999999998</v>
-      </c>
-      <c r="G28">
-        <v>2.33454E-3</v>
-      </c>
-      <c r="H28">
-        <v>38</v>
-      </c>
-      <c r="J28">
-        <v>26.611499999999999</v>
-      </c>
-      <c r="K28">
-        <v>1.84939E-3</v>
-      </c>
-      <c r="L28">
-        <v>27</v>
-      </c>
       <c r="N28">
         <v>2.7254100000000001</v>
       </c>
@@ -5033,24 +4587,6 @@
       <c r="D29">
         <v>8</v>
       </c>
-      <c r="F29">
-        <v>32.565800000000003</v>
-      </c>
-      <c r="G29">
-        <v>4.1046900000000002E-3</v>
-      </c>
-      <c r="H29">
-        <v>38</v>
-      </c>
-      <c r="J29">
-        <v>26.895900000000001</v>
-      </c>
-      <c r="K29">
-        <v>2.8679E-3</v>
-      </c>
-      <c r="L29">
-        <v>27</v>
-      </c>
       <c r="N29">
         <v>2.7131599999999998</v>
       </c>
@@ -5074,24 +4610,6 @@
       <c r="D30">
         <v>2</v>
       </c>
-      <c r="F30">
-        <v>3.4186000000000001</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>4</v>
-      </c>
-      <c r="J30">
-        <v>2.7674400000000001</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>3</v>
-      </c>
       <c r="N30">
         <v>2.10405</v>
       </c>
@@ -5115,24 +4633,6 @@
       <c r="D31">
         <v>8</v>
       </c>
-      <c r="F31">
-        <v>33.139499999999998</v>
-      </c>
-      <c r="G31">
-        <v>2.3419500000000002E-3</v>
-      </c>
-      <c r="H31">
-        <v>39</v>
-      </c>
-      <c r="J31">
-        <v>27.761600000000001</v>
-      </c>
-      <c r="K31">
-        <v>2.7350400000000002E-3</v>
-      </c>
-      <c r="L31">
-        <v>28</v>
-      </c>
       <c r="N31">
         <v>2.6993999999999998</v>
       </c>
@@ -5156,24 +4656,6 @@
       <c r="D32">
         <v>8</v>
       </c>
-      <c r="F32">
-        <v>33.131900000000002</v>
-      </c>
-      <c r="G32">
-        <v>2.3382300000000002E-3</v>
-      </c>
-      <c r="H32">
-        <v>39</v>
-      </c>
-      <c r="J32">
-        <v>27.755299999999998</v>
-      </c>
-      <c r="K32">
-        <v>2.9703300000000002E-3</v>
-      </c>
-      <c r="L32">
-        <v>28</v>
-      </c>
       <c r="N32">
         <v>2.6877399999999998</v>
       </c>
@@ -5197,24 +4679,6 @@
       <c r="D33">
         <v>8</v>
       </c>
-      <c r="F33">
-        <v>28.330200000000001</v>
-      </c>
-      <c r="G33">
-        <v>3.4384799999999998E-3</v>
-      </c>
-      <c r="H33">
-        <v>29</v>
-      </c>
-      <c r="J33">
-        <v>28.620799999999999</v>
-      </c>
-      <c r="K33">
-        <v>3.2284599999999998E-3</v>
-      </c>
-      <c r="L33">
-        <v>29</v>
-      </c>
       <c r="N33">
         <v>2.6749999999999998</v>
       </c>
@@ -5238,24 +4702,6 @@
       <c r="D34">
         <v>8</v>
       </c>
-      <c r="F34">
-        <v>34.279299999999999</v>
-      </c>
-      <c r="G34">
-        <v>3.6271400000000001E-3</v>
-      </c>
-      <c r="H34">
-        <v>40</v>
-      </c>
-      <c r="J34">
-        <v>28.905000000000001</v>
-      </c>
-      <c r="K34">
-        <v>3.8539999999999998E-3</v>
-      </c>
-      <c r="L34">
-        <v>29</v>
-      </c>
       <c r="N34">
         <v>2.6637499999999998</v>
       </c>
@@ -5279,24 +4725,6 @@
       <c r="D35">
         <v>8</v>
       </c>
-      <c r="F35">
-        <v>34.852899999999998</v>
-      </c>
-      <c r="G35">
-        <v>3.1136200000000001E-3</v>
-      </c>
-      <c r="H35">
-        <v>41</v>
-      </c>
-      <c r="J35">
-        <v>28.6084</v>
-      </c>
-      <c r="K35">
-        <v>3.3325300000000002E-3</v>
-      </c>
-      <c r="L35">
-        <v>29</v>
-      </c>
       <c r="N35">
         <v>2.6519400000000002</v>
       </c>
@@ -5320,24 +4748,6 @@
       <c r="D36">
         <v>8</v>
       </c>
-      <c r="F36">
-        <v>34.700499999999998</v>
-      </c>
-      <c r="G36">
-        <v>3.94028E-3</v>
-      </c>
-      <c r="H36">
-        <v>41</v>
-      </c>
-      <c r="J36">
-        <v>28.892900000000001</v>
-      </c>
-      <c r="K36">
-        <v>2.1584400000000002E-3</v>
-      </c>
-      <c r="L36">
-        <v>29</v>
-      </c>
       <c r="N36">
         <v>2.6429</v>
       </c>
@@ -5361,24 +4771,6 @@
       <c r="D37">
         <v>8</v>
       </c>
-      <c r="F37">
-        <v>35.564500000000002</v>
-      </c>
-      <c r="G37">
-        <v>5.3139900000000002E-3</v>
-      </c>
-      <c r="H37">
-        <v>42</v>
-      </c>
-      <c r="J37">
-        <v>29.758099999999999</v>
-      </c>
-      <c r="K37">
-        <v>2.2798800000000002E-3</v>
-      </c>
-      <c r="L37">
-        <v>30</v>
-      </c>
       <c r="N37">
         <v>2.6318999999999999</v>
       </c>
@@ -5402,24 +4794,6 @@
       <c r="D38">
         <v>8</v>
       </c>
-      <c r="F38">
-        <v>35.847799999999999</v>
-      </c>
-      <c r="G38">
-        <v>4.7124999999999997E-3</v>
-      </c>
-      <c r="H38">
-        <v>42</v>
-      </c>
-      <c r="J38">
-        <v>30.9133</v>
-      </c>
-      <c r="K38">
-        <v>4.8118800000000002E-3</v>
-      </c>
-      <c r="L38">
-        <v>31</v>
-      </c>
       <c r="N38">
         <v>2.6216599999999999</v>
       </c>
@@ -5443,24 +4817,6 @@
       <c r="D39">
         <v>8</v>
       </c>
-      <c r="F39">
-        <v>35.695799999999998</v>
-      </c>
-      <c r="G39">
-        <v>2.0116700000000001E-3</v>
-      </c>
-      <c r="H39">
-        <v>41</v>
-      </c>
-      <c r="J39">
-        <v>30.617100000000001</v>
-      </c>
-      <c r="K39">
-        <v>4.4358599999999998E-3</v>
-      </c>
-      <c r="L39">
-        <v>31</v>
-      </c>
       <c r="N39">
         <v>2.6114299999999999</v>
       </c>
@@ -5484,24 +4840,6 @@
       <c r="D40">
         <v>8</v>
       </c>
-      <c r="F40">
-        <v>36.559600000000003</v>
-      </c>
-      <c r="G40">
-        <v>2.8498E-3</v>
-      </c>
-      <c r="H40">
-        <v>43</v>
-      </c>
-      <c r="J40">
-        <v>30.901599999999998</v>
-      </c>
-      <c r="K40">
-        <v>1.72404E-3</v>
-      </c>
-      <c r="L40">
-        <v>31</v>
-      </c>
       <c r="N40">
         <v>2.60162</v>
       </c>
@@ -5525,24 +4863,6 @@
       <c r="D41">
         <v>2</v>
       </c>
-      <c r="F41">
-        <v>3.36</v>
-      </c>
-      <c r="G41">
-        <v>0</v>
-      </c>
-      <c r="H41">
-        <v>4</v>
-      </c>
-      <c r="J41">
-        <v>3.04</v>
-      </c>
-      <c r="K41">
-        <v>0</v>
-      </c>
-      <c r="L41">
-        <v>3</v>
-      </c>
       <c r="N41">
         <v>1.9697</v>
       </c>
@@ -5566,24 +4886,6 @@
       <c r="D42">
         <v>8</v>
       </c>
-      <c r="F42">
-        <v>37.278199999999998</v>
-      </c>
-      <c r="G42">
-        <v>5.8065299999999999E-3</v>
-      </c>
-      <c r="H42">
-        <v>44</v>
-      </c>
-      <c r="J42">
-        <v>30.605799999999999</v>
-      </c>
-      <c r="K42">
-        <v>4.20886E-3</v>
-      </c>
-      <c r="L42">
-        <v>31</v>
-      </c>
       <c r="N42">
         <v>2.5920999999999998</v>
       </c>
@@ -5607,24 +4909,6 @@
       <c r="D43">
         <v>8</v>
       </c>
-      <c r="F43">
-        <v>37.706600000000002</v>
-      </c>
-      <c r="G43">
-        <v>6.0604099999999996E-3</v>
-      </c>
-      <c r="H43">
-        <v>44</v>
-      </c>
-      <c r="J43">
-        <v>30.8904</v>
-      </c>
-      <c r="K43">
-        <v>2.6003599999999999E-3</v>
-      </c>
-      <c r="L43">
-        <v>31</v>
-      </c>
       <c r="N43">
         <v>2.5826799999999999</v>
       </c>
@@ -5648,24 +4932,6 @@
       <c r="D44">
         <v>8</v>
       </c>
-      <c r="F44">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="G44">
-        <v>5.6127599999999996E-3</v>
-      </c>
-      <c r="H44">
-        <v>44</v>
-      </c>
-      <c r="J44">
-        <v>31.754999999999999</v>
-      </c>
-      <c r="K44">
-        <v>4.76138E-3</v>
-      </c>
-      <c r="L44">
-        <v>32</v>
-      </c>
       <c r="N44">
         <v>2.5738099999999999</v>
       </c>
@@ -5689,24 +4955,6 @@
       <c r="D45">
         <v>8</v>
       </c>
-      <c r="F45">
-        <v>38.273499999999999</v>
-      </c>
-      <c r="G45">
-        <v>3.1361599999999998E-3</v>
-      </c>
-      <c r="H45">
-        <v>45</v>
-      </c>
-      <c r="J45">
-        <v>32.909399999999998</v>
-      </c>
-      <c r="K45">
-        <v>2.87601E-3</v>
-      </c>
-      <c r="L45">
-        <v>33</v>
-      </c>
       <c r="N45">
         <v>2.5647600000000002</v>
       </c>
@@ -5730,24 +4978,6 @@
       <c r="D46">
         <v>8</v>
       </c>
-      <c r="F46">
-        <v>39.136800000000001</v>
-      </c>
-      <c r="G46">
-        <v>6.5000700000000002E-3</v>
-      </c>
-      <c r="H46">
-        <v>46</v>
-      </c>
-      <c r="J46">
-        <v>32.613999999999997</v>
-      </c>
-      <c r="K46">
-        <v>2.9645100000000001E-3</v>
-      </c>
-      <c r="L46">
-        <v>33</v>
-      </c>
       <c r="N46">
         <v>2.5564800000000001</v>
       </c>
@@ -5771,24 +5001,6 @@
       <c r="D47">
         <v>8</v>
       </c>
-      <c r="F47">
-        <v>39.420299999999997</v>
-      </c>
-      <c r="G47">
-        <v>3.8347699999999999E-3</v>
-      </c>
-      <c r="H47">
-        <v>46</v>
-      </c>
-      <c r="J47">
-        <v>32.898600000000002</v>
-      </c>
-      <c r="K47">
-        <v>3.1726599999999999E-3</v>
-      </c>
-      <c r="L47">
-        <v>33</v>
-      </c>
       <c r="N47">
         <v>2.5489299999999999</v>
       </c>
@@ -5812,24 +5024,6 @@
       <c r="D48">
         <v>8</v>
       </c>
-      <c r="F48">
-        <v>39.993600000000001</v>
-      </c>
-      <c r="G48">
-        <v>3.9754500000000002E-3</v>
-      </c>
-      <c r="H48">
-        <v>47</v>
-      </c>
-      <c r="J48">
-        <v>32.603499999999997</v>
-      </c>
-      <c r="K48">
-        <v>3.1824499999999999E-3</v>
-      </c>
-      <c r="L48">
-        <v>33</v>
-      </c>
       <c r="N48">
         <v>2.5411899999999998</v>
       </c>
@@ -5853,24 +5047,6 @@
       <c r="D49">
         <v>8</v>
       </c>
-      <c r="F49">
-        <v>39.987400000000001</v>
-      </c>
-      <c r="G49">
-        <v>4.0384799999999997E-3</v>
-      </c>
-      <c r="H49">
-        <v>47</v>
-      </c>
-      <c r="J49">
-        <v>32.888199999999998</v>
-      </c>
-      <c r="K49">
-        <v>2.0107300000000001E-3</v>
-      </c>
-      <c r="L49">
-        <v>33</v>
-      </c>
       <c r="N49">
         <v>2.5327500000000001</v>
       </c>
@@ -5894,24 +5070,6 @@
       <c r="D50">
         <v>8</v>
       </c>
-      <c r="F50">
-        <v>40.705599999999997</v>
-      </c>
-      <c r="G50">
-        <v>2.5138199999999999E-3</v>
-      </c>
-      <c r="H50">
-        <v>48</v>
-      </c>
-      <c r="J50">
-        <v>33.752299999999998</v>
-      </c>
-      <c r="K50">
-        <v>2.9666699999999998E-3</v>
-      </c>
-      <c r="L50">
-        <v>34</v>
-      </c>
       <c r="N50">
         <v>2.5255200000000002</v>
       </c>
@@ -5935,24 +5093,6 @@
       <c r="D51">
         <v>8</v>
       </c>
-      <c r="F51">
-        <v>41.134099999999997</v>
-      </c>
-      <c r="G51">
-        <v>3.4546199999999998E-3</v>
-      </c>
-      <c r="H51">
-        <v>48</v>
-      </c>
-      <c r="J51">
-        <v>34.905999999999999</v>
-      </c>
-      <c r="K51">
-        <v>3.5216700000000002E-3</v>
-      </c>
-      <c r="L51">
-        <v>35</v>
-      </c>
       <c r="N51">
         <v>2.5173800000000002</v>
       </c>
@@ -5976,24 +5116,6 @@
       <c r="D52">
         <v>2</v>
       </c>
-      <c r="F52">
-        <v>3.4736799999999999</v>
-      </c>
-      <c r="G52">
-        <v>1.40345E-4</v>
-      </c>
-      <c r="H52">
-        <v>4</v>
-      </c>
-      <c r="J52">
-        <v>3.9473699999999998</v>
-      </c>
-      <c r="K52">
-        <v>0</v>
-      </c>
-      <c r="L52">
-        <v>4</v>
-      </c>
       <c r="N52">
         <v>1.91489</v>
       </c>
@@ -6017,24 +5139,6 @@
       <c r="D53">
         <v>8</v>
       </c>
-      <c r="F53">
-        <v>41.5625</v>
-      </c>
-      <c r="G53">
-        <v>3.5471399999999998E-3</v>
-      </c>
-      <c r="H53">
-        <v>49</v>
-      </c>
-      <c r="J53">
-        <v>34.6113</v>
-      </c>
-      <c r="K53">
-        <v>3.1515699999999998E-3</v>
-      </c>
-      <c r="L53">
-        <v>35</v>
-      </c>
       <c r="N53">
         <v>2.5106099999999998</v>
       </c>
@@ -6058,24 +5162,6 @@
       <c r="D54">
         <v>8</v>
       </c>
-      <c r="F54">
-        <v>41.7014</v>
-      </c>
-      <c r="G54">
-        <v>3.72544E-3</v>
-      </c>
-      <c r="H54">
-        <v>49</v>
-      </c>
-      <c r="J54">
-        <v>34.895899999999997</v>
-      </c>
-      <c r="K54">
-        <v>4.1632500000000003E-3</v>
-      </c>
-      <c r="L54">
-        <v>35</v>
-      </c>
       <c r="N54">
         <v>2.5027499999999998</v>
       </c>
@@ -6099,24 +5185,6 @@
       <c r="D55">
         <v>8</v>
       </c>
-      <c r="F55">
-        <v>42.5642</v>
-      </c>
-      <c r="G55">
-        <v>3.8939500000000002E-3</v>
-      </c>
-      <c r="H55">
-        <v>50</v>
-      </c>
-      <c r="J55">
-        <v>34.601500000000001</v>
-      </c>
-      <c r="K55">
-        <v>5.9331999999999996E-3</v>
-      </c>
-      <c r="L55">
-        <v>35</v>
-      </c>
       <c r="N55">
         <v>2.4964200000000001</v>
       </c>
@@ -6140,24 +5208,6 @@
       <c r="D56">
         <v>8</v>
       </c>
-      <c r="F56">
-        <v>42.703099999999999</v>
-      </c>
-      <c r="G56">
-        <v>4.5454199999999997E-3</v>
-      </c>
-      <c r="H56">
-        <v>50</v>
-      </c>
-      <c r="J56">
-        <v>34.886299999999999</v>
-      </c>
-      <c r="K56">
-        <v>5.1174799999999998E-3</v>
-      </c>
-      <c r="L56">
-        <v>35</v>
-      </c>
       <c r="N56">
         <v>2.48875</v>
       </c>
@@ -6181,24 +5231,6 @@
       <c r="D57">
         <v>8</v>
       </c>
-      <c r="F57">
-        <v>43.420999999999999</v>
-      </c>
-      <c r="G57">
-        <v>5.6533099999999999E-3</v>
-      </c>
-      <c r="H57">
-        <v>51</v>
-      </c>
-      <c r="J57">
-        <v>35.75</v>
-      </c>
-      <c r="K57">
-        <v>3.4178400000000001E-3</v>
-      </c>
-      <c r="L57">
-        <v>36</v>
-      </c>
       <c r="N57">
         <v>2.4828199999999998</v>
       </c>
@@ -6222,24 +5254,6 @@
       <c r="D58">
         <v>9</v>
       </c>
-      <c r="F58">
-        <v>44.234999999999999</v>
-      </c>
-      <c r="G58">
-        <v>7.5892299999999998E-3</v>
-      </c>
-      <c r="H58">
-        <v>52</v>
-      </c>
-      <c r="J58">
-        <v>36.693300000000001</v>
-      </c>
-      <c r="K58">
-        <v>3.6221299999999999E-3</v>
-      </c>
-      <c r="L58">
-        <v>37</v>
-      </c>
       <c r="N58">
         <v>2.6781299999999999</v>
       </c>
@@ -6263,24 +5277,6 @@
       <c r="D59">
         <v>3</v>
       </c>
-      <c r="F59">
-        <v>5.0406500000000003</v>
-      </c>
-      <c r="G59">
-        <v>0</v>
-      </c>
-      <c r="H59">
-        <v>6</v>
-      </c>
-      <c r="J59">
-        <v>4.87805</v>
-      </c>
-      <c r="K59">
-        <v>0</v>
-      </c>
-      <c r="L59">
-        <v>5</v>
-      </c>
       <c r="N59">
         <v>2.3164400000000001</v>
       </c>
@@ -6304,24 +5300,6 @@
       <c r="D60">
         <v>3</v>
       </c>
-      <c r="F60">
-        <v>5.8235299999999999</v>
-      </c>
-      <c r="G60">
-        <v>1.4012200000000001E-4</v>
-      </c>
-      <c r="H60">
-        <v>7</v>
-      </c>
-      <c r="J60">
-        <v>5.6617699999999997</v>
-      </c>
-      <c r="K60">
-        <v>1.10449E-4</v>
-      </c>
-      <c r="L60">
-        <v>6</v>
-      </c>
       <c r="N60">
         <v>2.4816500000000001</v>
       </c>
@@ -6345,24 +5323,6 @@
       <c r="D61">
         <v>3</v>
       </c>
-      <c r="F61">
-        <v>5.6</v>
-      </c>
-      <c r="G61">
-        <v>1.9851299999999999E-4</v>
-      </c>
-      <c r="H61">
-        <v>7</v>
-      </c>
-      <c r="J61">
-        <v>7.2</v>
-      </c>
-      <c r="K61">
-        <v>1.2705099999999999E-4</v>
-      </c>
-      <c r="L61">
-        <v>7</v>
-      </c>
       <c r="N61">
         <v>3.22255</v>
       </c>
@@ -6386,24 +5346,6 @@
       <c r="D62">
         <v>3</v>
       </c>
-      <c r="F62">
-        <v>6.6585400000000003</v>
-      </c>
-      <c r="G62">
-        <v>2.04787E-4</v>
-      </c>
-      <c r="H62">
-        <v>8</v>
-      </c>
-      <c r="J62">
-        <v>6.8170700000000002</v>
-      </c>
-      <c r="K62">
-        <v>2.6303900000000001E-4</v>
-      </c>
-      <c r="L62">
-        <v>7</v>
-      </c>
       <c r="N62">
         <v>2.9354800000000001</v>
       </c>
@@ -6427,24 +5369,6 @@
       <c r="D63">
         <v>4</v>
       </c>
-      <c r="F63">
-        <v>6.9213500000000003</v>
-      </c>
-      <c r="G63">
-        <v>1.3256699999999999E-4</v>
-      </c>
-      <c r="H63">
-        <v>8</v>
-      </c>
-      <c r="J63">
-        <v>7.0786499999999997</v>
-      </c>
-      <c r="K63">
-        <v>1.5391600000000001E-4</v>
-      </c>
-      <c r="L63">
-        <v>7</v>
-      </c>
       <c r="N63">
         <v>4.0885600000000002</v>
       </c>
@@ -6468,24 +5392,6 @@
       <c r="D64">
         <v>4</v>
       </c>
-      <c r="F64">
-        <v>7.5</v>
-      </c>
-      <c r="G64">
-        <v>1.7594099999999999E-4</v>
-      </c>
-      <c r="H64">
-        <v>9</v>
-      </c>
-      <c r="J64">
-        <v>7.96875</v>
-      </c>
-      <c r="K64">
-        <v>1.1276400000000001E-4</v>
-      </c>
-      <c r="L64">
-        <v>8</v>
-      </c>
       <c r="N64">
         <v>4.6675899999999997</v>
       </c>
@@ -6509,24 +5415,6 @@
       <c r="D65">
         <v>5</v>
       </c>
-      <c r="F65">
-        <v>7.4563100000000002</v>
-      </c>
-      <c r="G65">
-        <v>1.7526600000000001E-4</v>
-      </c>
-      <c r="H65">
-        <v>9</v>
-      </c>
-      <c r="J65">
-        <v>9.1650500000000008</v>
-      </c>
-      <c r="K65">
-        <v>2.0150300000000001E-4</v>
-      </c>
-      <c r="L65">
-        <v>9</v>
-      </c>
       <c r="N65">
         <v>6.0803599999999998</v>
       </c>
@@ -6550,24 +5438,6 @@
       <c r="D66">
         <v>11</v>
       </c>
-      <c r="F66">
-        <v>7.4181800000000004</v>
-      </c>
-      <c r="G66">
-        <v>1.8281300000000001E-4</v>
-      </c>
-      <c r="H66">
-        <v>8</v>
-      </c>
-      <c r="J66">
-        <v>8.8090899999999994</v>
-      </c>
-      <c r="K66">
-        <v>2.1692900000000001E-4</v>
-      </c>
-      <c r="L66">
-        <v>9</v>
-      </c>
       <c r="N66">
         <v>10.6334</v>
       </c>
@@ -6591,24 +5461,6 @@
       <c r="D67">
         <v>11</v>
       </c>
-      <c r="F67">
-        <v>8.6153899999999997</v>
-      </c>
-      <c r="G67">
-        <v>2.0167300000000001E-4</v>
-      </c>
-      <c r="H67">
-        <v>10</v>
-      </c>
-      <c r="J67">
-        <v>9.0769199999999994</v>
-      </c>
-      <c r="K67">
-        <v>2.0204399999999999E-4</v>
-      </c>
-      <c r="L67">
-        <v>9</v>
-      </c>
       <c r="N67">
         <v>12.22</v>
       </c>
@@ -6632,24 +5484,6 @@
       <c r="D68">
         <v>7</v>
       </c>
-      <c r="F68">
-        <v>8.5806400000000007</v>
-      </c>
-      <c r="G68">
-        <v>4.2064000000000001E-4</v>
-      </c>
-      <c r="H68">
-        <v>10</v>
-      </c>
-      <c r="J68">
-        <v>8.7338699999999996</v>
-      </c>
-      <c r="K68">
-        <v>4.2511300000000002E-4</v>
-      </c>
-      <c r="L68">
-        <v>9</v>
-      </c>
       <c r="N68">
         <v>7.1110600000000002</v>
       </c>
@@ -6673,24 +5507,6 @@
       <c r="D69">
         <v>7</v>
       </c>
-      <c r="F69">
-        <v>8.2442700000000002</v>
-      </c>
-      <c r="G69">
-        <v>4.1343100000000002E-4</v>
-      </c>
-      <c r="H69">
-        <v>9</v>
-      </c>
-      <c r="J69">
-        <v>9.0076300000000007</v>
-      </c>
-      <c r="K69">
-        <v>4.32032E-4</v>
-      </c>
-      <c r="L69">
-        <v>9</v>
-      </c>
       <c r="N69">
         <v>6.8857299999999997</v>
       </c>
@@ -6714,24 +5530,6 @@
       <c r="D70">
         <v>7</v>
       </c>
-      <c r="F70">
-        <v>9.7391299999999994</v>
-      </c>
-      <c r="G70">
-        <v>2.4732699999999999E-4</v>
-      </c>
-      <c r="H70">
-        <v>11</v>
-      </c>
-      <c r="J70">
-        <v>9.8913100000000007</v>
-      </c>
-      <c r="K70">
-        <v>2.4704799999999998E-4</v>
-      </c>
-      <c r="L70">
-        <v>10</v>
-      </c>
       <c r="N70">
         <v>6.3924599999999998</v>
       </c>
@@ -6755,24 +5553,6 @@
       <c r="D71">
         <v>7</v>
       </c>
-      <c r="F71">
-        <v>10.1655</v>
-      </c>
-      <c r="G71">
-        <v>2.5309900000000001E-4</v>
-      </c>
-      <c r="H71">
-        <v>11</v>
-      </c>
-      <c r="J71">
-        <v>11.075900000000001</v>
-      </c>
-      <c r="K71">
-        <v>5.4110599999999997E-4</v>
-      </c>
-      <c r="L71">
-        <v>11</v>
-      </c>
       <c r="N71">
         <v>5.8516599999999999</v>
       </c>
@@ -6796,24 +5576,6 @@
       <c r="D72">
         <v>8</v>
       </c>
-      <c r="F72">
-        <v>10.8947</v>
-      </c>
-      <c r="G72">
-        <v>5.9589699999999996E-4</v>
-      </c>
-      <c r="H72">
-        <v>13</v>
-      </c>
-      <c r="J72">
-        <v>10.743399999999999</v>
-      </c>
-      <c r="K72">
-        <v>2.8566699999999997E-4</v>
-      </c>
-      <c r="L72">
-        <v>11</v>
-      </c>
       <c r="N72">
         <v>5.8264899999999997</v>
       </c>
@@ -6837,24 +5599,6 @@
       <c r="D73">
         <v>8</v>
       </c>
-      <c r="F73">
-        <v>10.867900000000001</v>
-      </c>
-      <c r="G73">
-        <v>6.2648200000000004E-4</v>
-      </c>
-      <c r="H73">
-        <v>13</v>
-      </c>
-      <c r="J73">
-        <v>11.0189</v>
-      </c>
-      <c r="K73">
-        <v>3.0199300000000002E-4</v>
-      </c>
-      <c r="L73">
-        <v>11</v>
-      </c>
       <c r="N73">
         <v>5.4010800000000003</v>
       </c>
@@ -6878,24 +5622,6 @@
       <c r="D74">
         <v>8</v>
       </c>
-      <c r="F74">
-        <v>11.596399999999999</v>
-      </c>
-      <c r="G74">
-        <v>3.4517700000000001E-4</v>
-      </c>
-      <c r="H74">
-        <v>14</v>
-      </c>
-      <c r="J74">
-        <v>10.6928</v>
-      </c>
-      <c r="K74">
-        <v>3.0464000000000001E-4</v>
-      </c>
-      <c r="L74">
-        <v>11</v>
-      </c>
       <c r="N74">
         <v>5.1482700000000001</v>
       </c>
@@ -6919,24 +5645,6 @@
       <c r="D75">
         <v>8</v>
       </c>
-      <c r="F75">
-        <v>12.023099999999999</v>
-      </c>
-      <c r="G75">
-        <v>3.5528399999999998E-4</v>
-      </c>
-      <c r="H75">
-        <v>14</v>
-      </c>
-      <c r="J75">
-        <v>10.9711</v>
-      </c>
-      <c r="K75">
-        <v>3.1389200000000002E-4</v>
-      </c>
-      <c r="L75">
-        <v>11</v>
-      </c>
       <c r="N75">
         <v>5.0330300000000001</v>
       </c>
@@ -6960,24 +5668,6 @@
       <c r="D76">
         <v>8</v>
       </c>
-      <c r="F76">
-        <v>12.6</v>
-      </c>
-      <c r="G76">
-        <v>3.9130700000000003E-4</v>
-      </c>
-      <c r="H76">
-        <v>15</v>
-      </c>
-      <c r="J76">
-        <v>11.85</v>
-      </c>
-      <c r="K76">
-        <v>6.9714400000000002E-4</v>
-      </c>
-      <c r="L76">
-        <v>12</v>
-      </c>
       <c r="N76">
         <v>4.8232400000000002</v>
       </c>
@@ -7001,24 +5691,6 @@
       <c r="D77">
         <v>8</v>
       </c>
-      <c r="F77">
-        <v>12.4278</v>
-      </c>
-      <c r="G77">
-        <v>8.0323299999999999E-4</v>
-      </c>
-      <c r="H77">
-        <v>15</v>
-      </c>
-      <c r="J77">
-        <v>11.828900000000001</v>
-      </c>
-      <c r="K77">
-        <v>3.9145100000000002E-4</v>
-      </c>
-      <c r="L77">
-        <v>12</v>
-      </c>
       <c r="N77">
         <v>4.7285500000000003</v>
       </c>
@@ -7042,24 +5714,6 @@
       <c r="D78">
         <v>8</v>
       </c>
-      <c r="F78">
-        <v>13.3041</v>
-      </c>
-      <c r="G78">
-        <v>4.3666700000000001E-4</v>
-      </c>
-      <c r="H78">
-        <v>16</v>
-      </c>
-      <c r="J78">
-        <v>12.706200000000001</v>
-      </c>
-      <c r="K78">
-        <v>7.8760099999999997E-4</v>
-      </c>
-      <c r="L78">
-        <v>13</v>
-      </c>
       <c r="N78">
         <v>4.5528000000000004</v>
       </c>
@@ -7083,24 +5737,6 @@
       <c r="D79">
         <v>8</v>
       </c>
-      <c r="F79">
-        <v>13.582100000000001</v>
-      </c>
-      <c r="G79">
-        <v>4.3495799999999999E-4</v>
-      </c>
-      <c r="H79">
-        <v>16</v>
-      </c>
-      <c r="J79">
-        <v>12.985099999999999</v>
-      </c>
-      <c r="K79">
-        <v>2.8806399999999998E-4</v>
-      </c>
-      <c r="L79">
-        <v>13</v>
-      </c>
       <c r="N79">
         <v>4.4837800000000003</v>
       </c>
@@ -7124,24 +5760,6 @@
       <c r="D80">
         <v>8</v>
       </c>
-      <c r="F80">
-        <v>14.307700000000001</v>
-      </c>
-      <c r="G80">
-        <v>3.9191200000000001E-4</v>
-      </c>
-      <c r="H80">
-        <v>17</v>
-      </c>
-      <c r="J80">
-        <v>12.6683</v>
-      </c>
-      <c r="K80">
-        <v>6.8761400000000002E-4</v>
-      </c>
-      <c r="L80">
-        <v>13</v>
-      </c>
       <c r="N80">
         <v>4.3345799999999999</v>
       </c>
@@ -7165,24 +5783,6 @@
       <c r="D81">
         <v>8</v>
       </c>
-      <c r="F81">
-        <v>14.288399999999999</v>
-      </c>
-      <c r="G81">
-        <v>4.8998100000000001E-4</v>
-      </c>
-      <c r="H81">
-        <v>17</v>
-      </c>
-      <c r="J81">
-        <v>12.9488</v>
-      </c>
-      <c r="K81">
-        <v>4.45456E-4</v>
-      </c>
-      <c r="L81">
-        <v>13</v>
-      </c>
       <c r="N81">
         <v>4.2663399999999996</v>
       </c>
@@ -7206,24 +5806,6 @@
       <c r="D82">
         <v>8</v>
       </c>
-      <c r="F82">
-        <v>15.1622</v>
-      </c>
-      <c r="G82">
-        <v>1.0515500000000001E-3</v>
-      </c>
-      <c r="H82">
-        <v>18</v>
-      </c>
-      <c r="J82">
-        <v>13.824299999999999</v>
-      </c>
-      <c r="K82">
-        <v>4.9282299999999998E-4</v>
-      </c>
-      <c r="L82">
-        <v>14</v>
-      </c>
       <c r="N82">
         <v>4.1390200000000004</v>
       </c>
@@ -7247,24 +5829,6 @@
       <c r="D83">
         <v>8</v>
       </c>
-      <c r="F83">
-        <v>14.847200000000001</v>
-      </c>
-      <c r="G83">
-        <v>9.2164899999999997E-4</v>
-      </c>
-      <c r="H83">
-        <v>17</v>
-      </c>
-      <c r="J83">
-        <v>14.9956</v>
-      </c>
-      <c r="K83">
-        <v>5.15782E-4</v>
-      </c>
-      <c r="L83">
-        <v>15</v>
-      </c>
       <c r="N83">
         <v>4.0798699999999997</v>
       </c>
@@ -7288,24 +5852,6 @@
       <c r="D84">
         <v>8</v>
       </c>
-      <c r="F84">
-        <v>15.4237</v>
-      </c>
-      <c r="G84">
-        <v>1.04441E-3</v>
-      </c>
-      <c r="H84">
-        <v>18</v>
-      </c>
-      <c r="J84">
-        <v>14.6822</v>
-      </c>
-      <c r="K84">
-        <v>5.3412499999999999E-4</v>
-      </c>
-      <c r="L84">
-        <v>15</v>
-      </c>
       <c r="N84">
         <v>3.9703400000000002</v>
       </c>
@@ -7329,24 +5875,6 @@
       <c r="D85">
         <v>8</v>
       </c>
-      <c r="F85">
-        <v>16</v>
-      </c>
-      <c r="G85">
-        <v>1.0197400000000001E-3</v>
-      </c>
-      <c r="H85">
-        <v>19</v>
-      </c>
-      <c r="J85">
-        <v>14.962999999999999</v>
-      </c>
-      <c r="K85">
-        <v>9.3440099999999996E-4</v>
-      </c>
-      <c r="L85">
-        <v>15</v>
-      </c>
       <c r="N85">
         <v>3.91838</v>
       </c>
@@ -7370,24 +5898,6 @@
       <c r="D86">
         <v>8</v>
       </c>
-      <c r="F86">
-        <v>16.872</v>
-      </c>
-      <c r="G86">
-        <v>1.2708299999999999E-3</v>
-      </c>
-      <c r="H86">
-        <v>20</v>
-      </c>
-      <c r="J86">
-        <v>14.651999999999999</v>
-      </c>
-      <c r="K86">
-        <v>1.0853E-3</v>
-      </c>
-      <c r="L86">
-        <v>15</v>
-      </c>
       <c r="N86">
         <v>3.8234599999999999</v>
       </c>
@@ -7411,24 +5921,6 @@
       <c r="D87">
         <v>8</v>
       </c>
-      <c r="F87">
-        <v>17.151700000000002</v>
-      </c>
-      <c r="G87">
-        <v>1.2112E-3</v>
-      </c>
-      <c r="H87">
-        <v>20</v>
-      </c>
-      <c r="J87">
-        <v>14.9339</v>
-      </c>
-      <c r="K87">
-        <v>7.9065099999999996E-4</v>
-      </c>
-      <c r="L87">
-        <v>15</v>
-      </c>
       <c r="N87">
         <v>3.7765300000000002</v>
       </c>
@@ -7452,24 +5944,6 @@
       <c r="D88">
         <v>8</v>
       </c>
-      <c r="F88">
-        <v>17.7273</v>
-      </c>
-      <c r="G88">
-        <v>7.0152599999999995E-4</v>
-      </c>
-      <c r="H88">
-        <v>21</v>
-      </c>
-      <c r="J88">
-        <v>15.806800000000001</v>
-      </c>
-      <c r="K88">
-        <v>6.2219499999999997E-4</v>
-      </c>
-      <c r="L88">
-        <v>16</v>
-      </c>
       <c r="N88">
         <v>3.69381</v>
       </c>
@@ -7493,24 +5967,6 @@
       <c r="D89">
         <v>8</v>
       </c>
-      <c r="F89">
-        <v>17.712199999999999</v>
-      </c>
-      <c r="G89">
-        <v>9.4269299999999998E-4</v>
-      </c>
-      <c r="H89">
-        <v>21</v>
-      </c>
-      <c r="J89">
-        <v>16.9742</v>
-      </c>
-      <c r="K89">
-        <v>6.7296100000000002E-4</v>
-      </c>
-      <c r="L89">
-        <v>17</v>
-      </c>
       <c r="N89">
         <v>3.65829</v>
       </c>
@@ -7534,24 +5990,6 @@
       <c r="D90">
         <v>8</v>
       </c>
-      <c r="F90">
-        <v>18.287800000000001</v>
-      </c>
-      <c r="G90">
-        <v>8.5843599999999996E-4</v>
-      </c>
-      <c r="H90">
-        <v>21</v>
-      </c>
-      <c r="J90">
-        <v>16.665500000000002</v>
-      </c>
-      <c r="K90">
-        <v>7.7266599999999998E-4</v>
-      </c>
-      <c r="L90">
-        <v>17</v>
-      </c>
       <c r="N90">
         <v>3.5855899999999998</v>
       </c>
@@ -7575,24 +6013,6 @@
       <c r="D91">
         <v>8</v>
       </c>
-      <c r="F91">
-        <v>18.863199999999999</v>
-      </c>
-      <c r="G91">
-        <v>1.43739E-3</v>
-      </c>
-      <c r="H91">
-        <v>22</v>
-      </c>
-      <c r="J91">
-        <v>16.947399999999998</v>
-      </c>
-      <c r="K91">
-        <v>6.8633400000000003E-4</v>
-      </c>
-      <c r="L91">
-        <v>17</v>
-      </c>
       <c r="N91">
         <v>3.5477699999999999</v>
       </c>
@@ -7616,24 +6036,6 @@
       <c r="D92">
         <v>8</v>
       </c>
-      <c r="F92">
-        <v>19.2911</v>
-      </c>
-      <c r="G92">
-        <v>1.60618E-3</v>
-      </c>
-      <c r="H92">
-        <v>23</v>
-      </c>
-      <c r="J92">
-        <v>16.6404</v>
-      </c>
-      <c r="K92">
-        <v>1.4014400000000001E-3</v>
-      </c>
-      <c r="L92">
-        <v>17</v>
-      </c>
       <c r="N92">
         <v>3.4837600000000002</v>
       </c>
@@ -7657,24 +6059,6 @@
       <c r="D93">
         <v>8</v>
       </c>
-      <c r="F93">
-        <v>19.424700000000001</v>
-      </c>
-      <c r="G93">
-        <v>1.5460999999999999E-3</v>
-      </c>
-      <c r="H93">
-        <v>23</v>
-      </c>
-      <c r="J93">
-        <v>16.923100000000002</v>
-      </c>
-      <c r="K93">
-        <v>7.1496400000000001E-4</v>
-      </c>
-      <c r="L93">
-        <v>17</v>
-      </c>
       <c r="N93">
         <v>3.4495800000000001</v>
       </c>
@@ -7698,24 +6082,6 @@
       <c r="D94">
         <v>1</v>
       </c>
-      <c r="F94">
-        <v>2</v>
-      </c>
-      <c r="G94">
-        <v>0</v>
-      </c>
-      <c r="H94">
-        <v>2</v>
-      </c>
-      <c r="J94">
-        <v>2.1818200000000001</v>
-      </c>
-      <c r="K94">
-        <v>0</v>
-      </c>
-      <c r="L94">
-        <v>2</v>
-      </c>
       <c r="N94">
         <v>1.1764699999999999</v>
       </c>
@@ -7739,24 +6105,6 @@
       <c r="D95">
         <v>8</v>
       </c>
-      <c r="F95">
-        <v>20.2941</v>
-      </c>
-      <c r="G95">
-        <v>1.5259500000000001E-3</v>
-      </c>
-      <c r="H95">
-        <v>24</v>
-      </c>
-      <c r="J95">
-        <v>17.7941</v>
-      </c>
-      <c r="K95">
-        <v>1.5485900000000001E-3</v>
-      </c>
-      <c r="L95">
-        <v>18</v>
-      </c>
       <c r="N95">
         <v>3.3929399999999998</v>
       </c>
@@ -7780,24 +6128,6 @@
       <c r="D96">
         <v>8</v>
       </c>
-      <c r="F96">
-        <v>17.782699999999998</v>
-      </c>
-      <c r="G96">
-        <v>7.3459600000000001E-4</v>
-      </c>
-      <c r="H96">
-        <v>19</v>
-      </c>
-      <c r="J96">
-        <v>18.958500000000001</v>
-      </c>
-      <c r="K96">
-        <v>1.6672200000000001E-3</v>
-      </c>
-      <c r="L96">
-        <v>19</v>
-      </c>
       <c r="N96">
         <v>3.3618800000000002</v>
       </c>
@@ -7821,24 +6151,6 @@
       <c r="D97">
         <v>8</v>
       </c>
-      <c r="F97">
-        <v>20.856300000000001</v>
-      </c>
-      <c r="G97">
-        <v>1.86784E-3</v>
-      </c>
-      <c r="H97">
-        <v>24</v>
-      </c>
-      <c r="J97">
-        <v>18.653099999999998</v>
-      </c>
-      <c r="K97">
-        <v>8.6889699999999999E-4</v>
-      </c>
-      <c r="L97">
-        <v>19</v>
-      </c>
       <c r="N97">
         <v>3.3115199999999998</v>
       </c>
@@ -7862,24 +6174,6 @@
       <c r="D98">
         <v>8</v>
       </c>
-      <c r="F98">
-        <v>21.137599999999999</v>
-      </c>
-      <c r="G98">
-        <v>9.7144899999999999E-4</v>
-      </c>
-      <c r="H98">
-        <v>25</v>
-      </c>
-      <c r="J98">
-        <v>18.9358</v>
-      </c>
-      <c r="K98">
-        <v>1.7064999999999999E-3</v>
-      </c>
-      <c r="L98">
-        <v>19</v>
-      </c>
       <c r="N98">
         <v>3.2831600000000001</v>
       </c>
@@ -7902,24 +6196,6 @@
       </c>
       <c r="D99">
         <v>8</v>
-      </c>
-      <c r="F99">
-        <v>22.152699999999999</v>
-      </c>
-      <c r="G99">
-        <v>1.06387E-3</v>
-      </c>
-      <c r="H99">
-        <v>26</v>
-      </c>
-      <c r="J99">
-        <v>18.631699999999999</v>
-      </c>
-      <c r="K99">
-        <v>1.64073E-3</v>
-      </c>
-      <c r="L99">
-        <v>19</v>
       </c>
       <c r="N99">
         <v>3.2381899999999999</v>
@@ -7947,7 +6223,7 @@
   <dimension ref="A1:P99"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:H99"/>
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12008,8 +10284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:P99"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16070,8 +14346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:P99"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20133,7 +18409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A73" workbookViewId="0">
       <selection activeCell="AX3" sqref="AX3:AZ99"/>
     </sheetView>
   </sheetViews>
@@ -32168,12 +30444,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="R1:T1"/>
     <mergeCell ref="AX1:AZ1"/>
     <mergeCell ref="Z1:AB1"/>
     <mergeCell ref="AD1:AF1"/>
@@ -32181,6 +30451,12 @@
     <mergeCell ref="AL1:AN1"/>
     <mergeCell ref="AP1:AR1"/>
     <mergeCell ref="AT1:AV1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="R1:T1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -32191,7 +30467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="Z3" sqref="Z3:AB99"/>
     </sheetView>
   </sheetViews>
@@ -38918,7 +37194,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB99"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Z2" sqref="Z2:AB2"/>
     </sheetView>
   </sheetViews>

</xml_diff>